<commit_message>
Changes to form validations
</commit_message>
<xml_diff>
--- a/test/sample_forms/Form-3CE-update.xlsx
+++ b/test/sample_forms/Form-3CE-update.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\base\forms\base-form-management\test\sample_forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D074C04-7DD3-495A-966B-C5C59D3F3526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4510291F-5BC4-42CF-B546-C07DCC2F9B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="JaUivJj1XpzVIsMUuIWG4pvRwNkhjECqAfRNMoS0pEzY8qCMrWJoKRkwK5J/dPq5W+eH0fv+0nU0ZPhh5rEo8w==" workbookSaltValue="WSrsrEWzygKOJ9WtcOLB6A==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="28680" yWindow="1140" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -171,9 +171,6 @@
     <t>ATF</t>
   </si>
   <si>
-    <t>FI</t>
-  </si>
-  <si>
     <t>DS</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>3CE-update</t>
+  </si>
+  <si>
+    <t>PR</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1313,7 @@
   <dimension ref="B1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1353,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
@@ -1526,7 +1526,7 @@
         <v>8</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H18" s="11"/>
     </row>
@@ -1602,14 +1602,14 @@
         <v>28</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="47" t="s">
         <v>17</v>
       </c>
       <c r="G25" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H25" s="11"/>
     </row>
@@ -1630,14 +1630,14 @@
         <v>7</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="44" t="s">
         <v>21</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H27" s="11"/>
     </row>
@@ -1647,7 +1647,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -1660,14 +1660,14 @@
         <v>29</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="48" t="s">
         <v>12</v>
       </c>
       <c r="G29" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H29" s="11"/>
     </row>
@@ -1677,7 +1677,7 @@
         <v>22</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -2175,41 +2175,41 @@
         <v>21</v>
       </c>
       <c r="H5" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="J5" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="K5" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="L5" s="24" t="s">
         <v>62</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>63</v>
       </c>
       <c r="M5" s="24"/>
       <c r="N5" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O5" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="Q5" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Q5" s="24" t="s">
+      <c r="R5" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="R5" s="24" t="s">
+      <c r="S5" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="S5" s="24" t="s">
+      <c r="T5" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="T5" s="24" t="s">
-        <v>69</v>
       </c>
       <c r="U5" s="24"/>
       <c r="V5" s="24"/>
@@ -2307,7 +2307,7 @@
         <v>5201000</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="34">
         <v>33</v>
@@ -2447,7 +2447,7 @@
         <v>5201001</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="37">
         <v>44</v>
@@ -2501,10 +2501,10 @@
         <v>5201002</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="38">
         <v>1</v>
@@ -2555,7 +2555,7 @@
         <v>5201003</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="37">
         <v>55</v>
@@ -2564,7 +2564,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="58">
         <v>2645.8429999999998</v>
@@ -2611,7 +2611,7 @@
         <v>5201004</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="37">
         <v>77</v>
@@ -2665,7 +2665,7 @@
         <v>5201055</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="37">
         <v>88</v>
@@ -2721,7 +2721,7 @@
         <v>5201056</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="37">
         <v>99</v>
@@ -2775,7 +2775,7 @@
         <v>5201057</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="38">
@@ -2829,7 +2829,7 @@
         <v>5201058</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="37">
         <v>-3</v>
@@ -2883,7 +2883,7 @@
         <v>5201059</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="38">
@@ -2937,10 +2937,10 @@
         <v>5201060</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" s="38"/>
       <c r="G16" s="39"/>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="N16" s="59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O16" s="59">
         <v>0</v>
@@ -2989,11 +2989,11 @@
         <v>5201061</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G17" s="39">
         <v>600</v>
@@ -3087,7 +3087,7 @@
         <v>6505060</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="38"/>

</xml_diff>